<commit_message>
Updated Source file and output file with new column.
</commit_message>
<xml_diff>
--- a/BackOrderReport.xlsx
+++ b/BackOrderReport.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
   <si>
     <t xml:space="preserve">Sales Order</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">Confirmed CTP</t>
   </si>
   <si>
-    <t xml:space="preserve">Lines</t>
+    <t xml:space="preserve">Line</t>
   </si>
   <si>
     <t xml:space="preserve">Order Balance</t>
@@ -59,58 +59,186 @@
     <t xml:space="preserve">Dropzone</t>
   </si>
   <si>
+    <t xml:space="preserve">03/03/2020 06:19:30 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/20/2020 01:15:52 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">TrimSaw</t>
   </si>
   <si>
+    <t xml:space="preserve">03/11/2020 10:13:40 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/05/2020 02:25:58 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/13/2020 01:14:04 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Machining</t>
   </si>
   <si>
+    <t xml:space="preserve">03/05/2020 01:29:10 PM</t>
+  </si>
+  <si>
     <t xml:space="preserve">B11314</t>
   </si>
   <si>
     <t xml:space="preserve">Amazon</t>
   </si>
   <si>
+    <t xml:space="preserve">03/05/2020 11:41:43 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/25/2020 07:02:58 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/12/2020 08:35:37 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/04/2020 04:06:42 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2020 05:29:57 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/15/2020 09:08:10 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/05/2020 11:54:00 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/02/2020 01:36:53 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">B11451</t>
   </si>
   <si>
     <t xml:space="preserve">Facebook</t>
   </si>
   <si>
+    <t xml:space="preserve">01/27/2020 02:34:54 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/06/2020 12:07:02 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/07/2020 06:22:30 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/17/2020 09:01:58 PM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wrap</t>
   </si>
   <si>
+    <t xml:space="preserve">03/05/2020 11:53:22 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/18/2020 09:40:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/07/2020 09:00:58 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2020 09:41:26 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/03/2020 10:33:53 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/08/2020 01:37:38 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/22/2020 04:57:42 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/22/2020 03:11:36 PM</t>
+  </si>
+  <si>
     <t xml:space="preserve">B11164</t>
   </si>
   <si>
     <t xml:space="preserve">Google</t>
   </si>
   <si>
+    <t xml:space="preserve">01/28/2020 09:24:37 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/03/2020 06:50:08 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/21/2020 07:11:07 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/14/2020 02:35:40 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/20/2020 09:12:31 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">B45646</t>
   </si>
   <si>
+    <t xml:space="preserve">02/06/2020 12:11:17 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/27/2020 11:03:49 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/27/2020 04:11:07 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">B65311</t>
   </si>
   <si>
     <t xml:space="preserve">CommaAI</t>
   </si>
   <si>
+    <t xml:space="preserve">01/27/2020 02:41:26 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/07/2020 08:15:21 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/04/2020 05:04:20 PM</t>
+  </si>
+  <si>
     <t xml:space="preserve">B84654</t>
   </si>
   <si>
     <t xml:space="preserve">Capital One</t>
   </si>
   <si>
+    <t xml:space="preserve">01/22/2020 10:19:47 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/06/2020 05:06:20 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">LayupCold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/04/2020 10:54:04 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/09/2020 07:48:54 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/25/2020 06:21:16 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -192,12 +320,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,18 +341,22 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -230,54 +366,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="21.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -304,6 +441,10 @@
       <c r="H2" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -330,6 +471,10 @@
       <c r="H3" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -354,8 +499,12 @@
         <v>5</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>12</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -382,6 +531,10 @@
       <c r="H5" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -408,6 +561,10 @@
       <c r="H6" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -432,15 +589,19 @@
         <v>8</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>43875</v>
@@ -460,13 +621,17 @@
       <c r="H8" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>43875</v>
@@ -486,13 +651,17 @@
       <c r="H9" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>43875</v>
@@ -512,13 +681,17 @@
       <c r="H10" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>43875</v>
@@ -536,15 +709,19 @@
         <v>10</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>12</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>43875</v>
@@ -564,13 +741,17 @@
       <c r="H12" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>43875</v>
@@ -590,13 +771,17 @@
       <c r="H13" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>43875</v>
@@ -616,13 +801,17 @@
       <c r="H14" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>43875</v>
@@ -642,13 +831,17 @@
       <c r="H15" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>43875</v>
@@ -668,13 +861,17 @@
       <c r="H16" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>43875</v>
@@ -694,13 +891,17 @@
       <c r="H17" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>43875</v>
@@ -720,13 +921,17 @@
       <c r="H18" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>43875</v>
@@ -746,13 +951,17 @@
       <c r="H19" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>43875</v>
@@ -770,15 +979,19 @@
         <v>4</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>18</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>43875</v>
@@ -796,15 +1009,19 @@
         <v>5</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>12</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>43875</v>
@@ -824,13 +1041,17 @@
       <c r="H22" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>43875</v>
@@ -850,13 +1071,17 @@
       <c r="H23" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>43875</v>
@@ -876,13 +1101,17 @@
       <c r="H24" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>43875</v>
@@ -902,13 +1131,17 @@
       <c r="H25" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>43875</v>
@@ -926,15 +1159,19 @@
         <v>1</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>43875</v>
@@ -954,13 +1191,17 @@
       <c r="H27" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>43875</v>
@@ -978,15 +1219,19 @@
         <v>5</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>18</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>43875</v>
@@ -1004,15 +1249,19 @@
         <v>4</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>43875</v>
@@ -1030,15 +1279,19 @@
         <v>1</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>12</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>43875</v>
@@ -1058,13 +1311,17 @@
       <c r="H31" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I31" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>43875</v>
@@ -1084,13 +1341,17 @@
       <c r="H32" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>43875</v>
@@ -1110,13 +1371,17 @@
       <c r="H33" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I33" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>43875</v>
@@ -1136,13 +1401,17 @@
       <c r="H34" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I34" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>43875</v>
@@ -1162,13 +1431,17 @@
       <c r="H35" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>43875</v>
@@ -1186,15 +1459,19 @@
         <v>1</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>12</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>43875</v>
@@ -1214,13 +1491,17 @@
       <c r="H37" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I37" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>43875</v>
@@ -1238,15 +1519,19 @@
         <v>8</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>43875</v>
@@ -1266,13 +1551,17 @@
       <c r="H39" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>43875</v>
@@ -1292,13 +1581,17 @@
       <c r="H40" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>43875</v>
@@ -1316,15 +1609,19 @@
         <v>6</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>26</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>43875</v>
@@ -1342,15 +1639,19 @@
         <v>1</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>12</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>43875</v>
@@ -1370,6 +1671,13 @@
       <c r="H43" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="I43" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I44" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1393,10 +1701,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>